<commit_message>
[FIX] Tratativa para erro de login
</commit_message>
<xml_diff>
--- a/Data/Parametrização de Mensagens.xlsx
+++ b/Data/Parametrização de Mensagens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_Oracle\dhl-dtentry-oracle\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A1E8003-3F63-4B22-AC7A-DCD7F9FB97E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C110AF0-E367-4EF2-87F1-A3BCB6E2C3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6198A0C9-7991-42CB-8E11-C2B8A56D157A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Msg RPA</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Msg PPD</t>
   </si>
   <si>
-    <t>[CANCELAR_PROCESSO]PROCESSO DESCONSIDERADO - Documento já lançado, favor verificar e nos contatar via e-mail caso o novo lançamento seja devido mesmo assim.</t>
-  </si>
-  <si>
     <t>O CNPJ do fornecedor (49930514000135) do documento não está cadastrado na Filial</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
   </si>
   <si>
     <t>O CNPJ do fornecedor (37153564000174) do documento não está cadastrado na Filial</t>
-  </si>
-  <si>
-    <t>Documento já lançado, favor verificar e nos contatar via e-mail caso o novo lançamento seja devido mesmo assim.</t>
   </si>
   <si>
     <t>[CANCELAR_PROCESSO]PROCESSO DESCONSIDERADO - O CNPJ do fornecedor (37153564000174) do documento não está cadastrado na Filial</t>
@@ -434,7 +428,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A5" sqref="A5:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -452,35 +446,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>

</xml_diff>

<commit_message>
[FIX] Ajuste na tela de linhas: add tratativa para preço unitário divergindo da PO não travar o robô.
</commit_message>
<xml_diff>
--- a/Data/Parametrização de Mensagens.xlsx
+++ b/Data/Parametrização de Mensagens.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa0DHLEARQ1\Documents\UiPath\RPA_Oracle\dhl-dtentry-oracle\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C110AF0-E367-4EF2-87F1-A3BCB6E2C3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E6FEDC-3DF6-4F2B-A2BB-9E5D073C2FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{6198A0C9-7991-42CB-8E11-C2B8A56D157A}"/>
   </bookViews>
@@ -427,9 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC6AD3F-C443-4E1B-9E2F-90F989BEEADB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>